<commit_message>
add thuât toán text
</commit_message>
<xml_diff>
--- a/TH Excel/5. Nội suy trung tâm/Nội suy trung tâm.xlsx
+++ b/TH Excel/5. Nội suy trung tâm/Nội suy trung tâm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtien\Desktop\PPS\Tien\5. Nội suy trung tâm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtien\Desktop\BK\PPS\Tien 20251\Numerical-Analysis\TH Excel\5. Nội suy trung tâm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D06157-E367-405D-A8E1-460F04FD61C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3052BA8D-D980-43C7-A2DE-FE7CE22E0E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{305B22B5-5178-4B87-8DF4-001635C2ED15}"/>
+    <workbookView xWindow="2970" yWindow="1260" windowWidth="14400" windowHeight="7270" firstSheet="1" activeTab="3" xr2:uid="{305B22B5-5178-4B87-8DF4-001635C2ED15}"/>
   </bookViews>
   <sheets>
     <sheet name="NS bessel" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -611,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,12 +663,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -676,12 +670,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,7 +1148,7 @@
         <v>117</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H2:H10" si="2">VLOOKUP(G3,B3:D203,2)</f>
+        <f t="shared" ref="H3:H10" si="2">VLOOKUP(G3,B3:D203,2)</f>
         <v>14.806000000000026</v>
       </c>
       <c r="I3" s="1">
@@ -1605,11 +1603,11 @@
         <f t="shared" si="0"/>
         <v>4.3769</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="24">
         <f>I6</f>
         <v>5.5758999999999999</v>
@@ -2351,11 +2349,11 @@
         <f t="shared" si="0"/>
         <v>1.2083999999999999</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
       <c r="I29" s="13">
         <f>I6</f>
         <v>5.5758999999999999</v>
@@ -5806,7 +5804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368E3BAF-E979-4C0B-81A5-53215E90B212}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -5828,7 +5826,7 @@
       <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>52</v>
       </c>
       <c r="E1">
@@ -5850,7 +5848,7 @@
       <c r="C2">
         <v>-3.0437400000000001</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="47" t="s">
         <v>53</v>
       </c>
       <c r="E2">
@@ -5868,7 +5866,7 @@
       <c r="C3">
         <v>-2.7483300000000002</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="47" t="s">
         <v>54</v>
       </c>
       <c r="E3">
@@ -6011,7 +6009,7 @@
         <v>2.4178099999999998</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K7:O12" si="2">J8-J7</f>
+        <f t="shared" ref="K8:O12" si="2">J8-J7</f>
         <v>0.9075899999999999</v>
       </c>
       <c r="L8">
@@ -6453,16 +6451,16 @@
       <c r="C28">
         <v>-3.63246</v>
       </c>
-      <c r="J28" s="50">
-        <v>0</v>
-      </c>
-      <c r="K28" s="51">
-        <v>0</v>
-      </c>
-      <c r="L28" s="51">
-        <v>0</v>
-      </c>
-      <c r="M28" s="52">
+      <c r="J28" s="48">
+        <v>0</v>
+      </c>
+      <c r="K28" s="49">
+        <v>0</v>
+      </c>
+      <c r="L28" s="49">
+        <v>0</v>
+      </c>
+      <c r="M28" s="50">
         <v>1</v>
       </c>
     </row>
@@ -6479,17 +6477,17 @@
       <c r="I29">
         <v>0.25</v>
       </c>
-      <c r="J29" s="53" cm="1">
+      <c r="J29" s="51" cm="1">
         <f t="array" ref="J29:M29">K28:N28-I29*J28:M28</f>
         <v>0</v>
       </c>
-      <c r="K29" s="54">
-        <v>0</v>
-      </c>
-      <c r="L29" s="54">
-        <v>1</v>
-      </c>
-      <c r="M29" s="55">
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" s="52">
         <v>-0.25</v>
       </c>
     </row>
@@ -6506,17 +6504,17 @@
       <c r="I30">
         <v>2.25</v>
       </c>
-      <c r="J30" s="53" cm="1">
+      <c r="J30" s="51" cm="1">
         <f t="array" ref="J30:M30">K29:N29-I30*J29:M29</f>
         <v>0</v>
       </c>
-      <c r="K30" s="54">
-        <v>1</v>
-      </c>
-      <c r="L30" s="54">
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
         <v>-2.5</v>
       </c>
-      <c r="M30" s="55">
+      <c r="M30" s="52">
         <v>0.5625</v>
       </c>
     </row>
@@ -6533,17 +6531,17 @@
       <c r="I31">
         <v>6.25</v>
       </c>
-      <c r="J31" s="56" cm="1">
+      <c r="J31" s="53" cm="1">
         <f t="array" ref="J31:M31">K30:N30-I31*J30:M30</f>
         <v>1</v>
       </c>
-      <c r="K31" s="57">
+      <c r="K31" s="54">
         <v>-8.75</v>
       </c>
-      <c r="L31" s="57">
+      <c r="L31" s="54">
         <v>16.1875</v>
       </c>
-      <c r="M31" s="58">
+      <c r="M31" s="55">
         <v>-3.515625</v>
       </c>
     </row>
@@ -6779,7 +6777,7 @@
         <v>3.2493370630642749E-5</v>
       </c>
       <c r="M42">
-        <f t="shared" ref="L42:Q42" si="3">L42*$I$42+M41</f>
+        <f t="shared" ref="M42:Q42" si="3">L42*$I$42+M41</f>
         <v>4.3215962280970528E-4</v>
       </c>
       <c r="N42">
@@ -6821,7 +6819,7 @@
         <v>-9.0751937257862458E-7</v>
       </c>
       <c r="L43">
-        <f t="shared" ref="L43:P43" si="4">$I$42*K43+L42</f>
+        <f t="shared" ref="L43:O43" si="4">$I$42*K43+L42</f>
         <v>3.2504089363389741E-5</v>
       </c>
       <c r="M43">
@@ -6836,7 +6834,7 @@
         <f t="shared" si="4"/>
         <v>-8.4451637288906825E-2</v>
       </c>
-      <c r="P43" s="59">
+      <c r="P43">
         <f>$I$42*O43+P42</f>
         <v>0.77131639684798503</v>
       </c>
@@ -11341,8 +11339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE404C4-8B46-48C4-8A54-9A6B10091A0E}">
   <dimension ref="B1:Y202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="P9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11619,11 +11617,11 @@
         <v>2.7957999999999998</v>
       </c>
       <c r="G6">
-        <f t="shared" si="5"/>
+        <f>G5+1</f>
         <v>120</v>
       </c>
       <c r="H6" s="17">
-        <f t="shared" si="1"/>
+        <f>VLOOKUP(G6,B6:D206,2)</f>
         <v>15.160000000000027</v>
       </c>
       <c r="I6" s="24">
@@ -11932,11 +11930,11 @@
         <f t="shared" si="0"/>
         <v>4.3769</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="24">
         <f>I6</f>
         <v>5.5758999999999999</v>
@@ -12678,11 +12676,11 @@
         <f t="shared" si="0"/>
         <v>1.2083999999999999</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
       <c r="I29" s="13">
         <f>I6</f>
         <v>5.5758999999999999</v>
@@ -15767,11 +15765,11 @@
         <f t="shared" si="0"/>
         <v>4.3769</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="24">
         <f>I6</f>
         <v>5.5377000000000001</v>
@@ -16267,11 +16265,11 @@
         <f t="shared" si="0"/>
         <v>1.2083999999999999</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
       <c r="I29" s="13">
         <f>I5</f>
         <v>5.5758999999999999</v>

</xml_diff>